<commit_message>
Update Valkyrie Duet 3 6HC Connection Table.xlsx
</commit_message>
<xml_diff>
--- a/Firmware/RRF/Valkyrie Duet 3 6HC Connection Table.xlsx
+++ b/Firmware/RRF/Valkyrie Duet 3 6HC Connection Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Firmware/RRF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{C788BE8B-89FF-47EE-BC54-747C3D562542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF85D5A8-66CB-4F32-A4FF-7C210BD47A2E}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="8_{C788BE8B-89FF-47EE-BC54-747C3D562542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12BD9C28-DB7F-4A44-AC59-98AD2AC84125}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{344B6B93-88E2-4E8A-A19A-9E2625195A37}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{344B6B93-88E2-4E8A-A19A-9E2625195A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>IO_3</t>
   </si>
   <si>
-    <t>io8.in</t>
-  </si>
-  <si>
     <t>DRIVER 2</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>Wire nr</t>
+  </si>
+  <si>
+    <t>io3.in</t>
   </si>
 </sst>
 </file>
@@ -777,7 +777,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -785,14 +785,14 @@
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>23</v>
@@ -804,7 +804,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
         <v>110</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
         <v>110</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>10</v>
@@ -891,7 +891,7 @@
         <v>110</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>11</v>
@@ -920,7 +920,7 @@
         <v>110</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -949,7 +949,7 @@
         <v>110</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
         <v>110</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1007,7 +1007,7 @@
         <v>110</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1036,7 +1036,7 @@
         <v>110</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1065,7 +1065,7 @@
         <v>110</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
         <v>110</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1123,7 +1123,7 @@
         <v>110</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
         <v>110</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
         <v>110</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
         <v>110</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1230,7 +1230,7 @@
         <v>40</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="G17" s="19">
         <v>24</v>
@@ -1239,7 +1239,7 @@
         <v>110</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1268,7 +1268,7 @@
         <v>110</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1285,11 +1285,11 @@
         <v>18</v>
       </c>
       <c r="E19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>43</v>
-      </c>
       <c r="G19" s="2">
         <v>24</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>110</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1314,10 +1314,10 @@
         <v>19</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G20" s="5">
         <v>24</v>
@@ -1326,7 +1326,7 @@
         <v>110</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1343,10 +1343,10 @@
         <v>20</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="2">
         <v>24</v>
@@ -1355,7 +1355,7 @@
         <v>110</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1372,10 +1372,10 @@
         <v>21</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G22" s="5">
         <v>24</v>
@@ -1384,7 +1384,7 @@
         <v>110</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1395,13 +1395,13 @@
         <v>21</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>28</v>
@@ -1413,7 +1413,7 @@
         <v>110</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1424,17 +1424,17 @@
         <v>22</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>48</v>
-      </c>
       <c r="G24" s="21">
         <v>24</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>110</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1453,16 +1453,16 @@
         <v>23</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G25" s="24">
         <v>24</v>
@@ -1471,7 +1471,7 @@
         <v>110</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1482,17 +1482,17 @@
         <v>24</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>56</v>
-      </c>
       <c r="G26" s="21">
         <v>24</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>110</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1511,13 +1511,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>37</v>
@@ -1529,7 +1529,7 @@
         <v>110</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1540,17 +1540,17 @@
         <v>26</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>60</v>
-      </c>
       <c r="G28" s="21">
         <v>24</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>110</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1569,13 +1569,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>28</v>
@@ -1587,7 +1587,7 @@
         <v>100</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1598,16 +1598,16 @@
         <v>28</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="21" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="G30" s="21">
         <v>24</v>
@@ -1616,7 +1616,7 @@
         <v>100</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1627,13 +1627,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>25</v>
@@ -1645,7 +1645,7 @@
         <v>50</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1656,16 +1656,16 @@
         <v>30</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D32" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G32" s="21">
         <v>24</v>
@@ -1674,7 +1674,7 @@
         <v>50</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1685,13 +1685,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>25</v>
@@ -1712,16 +1712,16 @@
         <v>32</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G34" s="21">
         <v>24</v>

</xml_diff>